<commit_message>
Update asset progress and chart data in Asset.html
Adjusted the progress bar value from 59% to 32% and updated the asset chart data with new dates and values for all datasets. Also updated the related Excel file with new data.
</commit_message>
<xml_diff>
--- a/article/家庭财务管理手册2025.xlsx
+++ b/article/家庭财务管理手册2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18717\Documents\GitHub\luyao.github.io\article\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76B8981-CBB3-4C04-AB29-CA68B75CD4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD091932-1563-4C71-A0F7-7D0523E5D70A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4622,6 +4622,39 @@
     <xf numFmtId="0" fontId="13" fillId="17" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="5" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4655,38 +4688,59 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4694,65 +4748,11 @@
     <xf numFmtId="10" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="9" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6345,6 +6345,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5908322.3900000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5822023.9699999988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8791,7 +8794,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -9079,8 +9082,8 @@
         <v>5908322.3900000006</v>
       </c>
       <c r="O12" s="191">
-        <f>(6500000-N12)/1000000</f>
-        <v>0.59167760999999941</v>
+        <f>(N12-5500000)/1000000</f>
+        <v>0.40832239000000059</v>
       </c>
     </row>
     <row r="13" spans="2:16" ht="24.65" customHeight="1">
@@ -9098,8 +9101,14 @@
       <c r="K13" s="137"/>
       <c r="L13" s="138"/>
       <c r="M13" s="141"/>
-      <c r="N13" s="138"/>
-      <c r="O13" s="191"/>
+      <c r="N13" s="138">
+        <f>'3、存量资产-y'!L26+'3、存量资产-k'!L13</f>
+        <v>5822023.9699999988</v>
+      </c>
+      <c r="O13" s="191">
+        <f>(N13-5500000)/1000000</f>
+        <v>0.32202396999999883</v>
+      </c>
     </row>
     <row r="14" spans="2:16" ht="25" customHeight="1">
       <c r="B14" s="132" t="s">
@@ -9219,7 +9228,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K21" sqref="K21"/>
+      <selection pane="bottomRight" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -9300,7 +9309,9 @@
       <c r="K2" s="119">
         <v>11978</v>
       </c>
-      <c r="L2" s="119"/>
+      <c r="L2" s="119">
+        <v>11585</v>
+      </c>
       <c r="M2" s="128"/>
     </row>
     <row r="3" spans="1:13" ht="20.5" customHeight="1">
@@ -9335,7 +9346,9 @@
       <c r="K3" s="120">
         <v>113137.2</v>
       </c>
-      <c r="L3" s="120"/>
+      <c r="L3" s="120">
+        <v>105966</v>
+      </c>
       <c r="M3" s="128"/>
     </row>
     <row r="4" spans="1:13" ht="20.5" customHeight="1">
@@ -9370,7 +9383,9 @@
       <c r="K4" s="119">
         <v>400</v>
       </c>
-      <c r="L4" s="119"/>
+      <c r="L4" s="119">
+        <v>0</v>
+      </c>
       <c r="M4" s="128"/>
     </row>
     <row r="5" spans="1:13" ht="20.5" customHeight="1">
@@ -9405,7 +9420,9 @@
       <c r="K5" s="120">
         <v>1000</v>
       </c>
-      <c r="L5" s="120"/>
+      <c r="L5" s="119">
+        <v>14792</v>
+      </c>
       <c r="M5" s="128"/>
     </row>
     <row r="6" spans="1:13" ht="20.5" customHeight="1">
@@ -9440,7 +9457,9 @@
       <c r="K6" s="119">
         <v>92764</v>
       </c>
-      <c r="L6" s="119"/>
+      <c r="L6" s="119">
+        <v>122464</v>
+      </c>
       <c r="M6" s="128"/>
     </row>
     <row r="7" spans="1:13" ht="20.5" customHeight="1">
@@ -9504,7 +9523,9 @@
       <c r="K8" s="119">
         <v>22367</v>
       </c>
-      <c r="L8" s="119"/>
+      <c r="L8" s="119">
+        <v>22171</v>
+      </c>
       <c r="M8" s="128"/>
     </row>
     <row r="9" spans="1:13" ht="20.5" customHeight="1">
@@ -9537,7 +9558,9 @@
       <c r="K9" s="119">
         <v>69.819999999999993</v>
       </c>
-      <c r="L9" s="119"/>
+      <c r="L9" s="119">
+        <v>5.65</v>
+      </c>
       <c r="M9" s="128"/>
     </row>
     <row r="10" spans="1:13" ht="20.5" customHeight="1">
@@ -9568,7 +9591,9 @@
       <c r="K10" s="119">
         <v>36564</v>
       </c>
-      <c r="L10" s="119"/>
+      <c r="L10" s="119">
+        <v>0</v>
+      </c>
       <c r="M10" s="128"/>
     </row>
     <row r="11" spans="1:13" ht="20.5" customHeight="1">
@@ -9679,7 +9704,9 @@
       <c r="K13" s="119">
         <v>20096</v>
       </c>
-      <c r="L13" s="119"/>
+      <c r="L13" s="119">
+        <v>20049</v>
+      </c>
       <c r="M13" s="128"/>
     </row>
     <row r="14" spans="1:13" ht="20.5" customHeight="1">
@@ -9708,7 +9735,9 @@
       <c r="K14" s="119">
         <v>395128</v>
       </c>
-      <c r="L14" s="119"/>
+      <c r="L14" s="119">
+        <v>394720</v>
+      </c>
       <c r="M14" s="128"/>
     </row>
     <row r="15" spans="1:13" ht="20.5" customHeight="1">
@@ -9735,7 +9764,9 @@
       <c r="K15" s="119">
         <v>32463</v>
       </c>
-      <c r="L15" s="119"/>
+      <c r="L15" s="119">
+        <v>32384</v>
+      </c>
       <c r="M15" s="128"/>
     </row>
     <row r="16" spans="1:13" ht="20.5" customHeight="1">
@@ -9762,7 +9793,9 @@
       <c r="K16" s="119">
         <v>102611</v>
       </c>
-      <c r="L16" s="119"/>
+      <c r="L16" s="119">
+        <v>102293</v>
+      </c>
       <c r="M16" s="128"/>
     </row>
     <row r="17" spans="1:13" ht="20.5" customHeight="1">
@@ -9810,8 +9843,8 @@
         <v>1828578.02</v>
       </c>
       <c r="L17" s="122">
-        <f t="shared" si="0"/>
-        <v>1000000</v>
+        <f>SUM(L2:L16)</f>
+        <v>1826429.65</v>
       </c>
       <c r="M17" s="128"/>
     </row>
@@ -9847,7 +9880,9 @@
       <c r="K18" s="119">
         <v>135290</v>
       </c>
-      <c r="L18" s="119"/>
+      <c r="L18" s="119">
+        <v>135584</v>
+      </c>
       <c r="M18" s="128"/>
     </row>
     <row r="19" spans="1:13" ht="20.5" customHeight="1">
@@ -9882,7 +9917,9 @@
       <c r="K19" s="119">
         <v>125649</v>
       </c>
-      <c r="L19" s="119"/>
+      <c r="L19" s="119">
+        <v>133109</v>
+      </c>
       <c r="M19" s="128"/>
     </row>
     <row r="20" spans="1:13" ht="20.5" customHeight="1">
@@ -9917,7 +9954,9 @@
       <c r="K20" s="120">
         <v>11395</v>
       </c>
-      <c r="L20" s="120"/>
+      <c r="L20" s="120">
+        <v>22888</v>
+      </c>
       <c r="M20" s="128"/>
     </row>
     <row r="21" spans="1:13" ht="20.5" customHeight="1">
@@ -9966,7 +10005,7 @@
       </c>
       <c r="L21" s="124">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>291581</v>
       </c>
       <c r="M21" s="128"/>
     </row>
@@ -10100,7 +10139,7 @@
       </c>
       <c r="L25" s="126">
         <f t="shared" si="3"/>
-        <v>1000000</v>
+        <v>2118010.65</v>
       </c>
       <c r="M25" s="128"/>
     </row>
@@ -10150,7 +10189,7 @@
       </c>
       <c r="L26" s="126">
         <f t="shared" si="4"/>
-        <v>1000000</v>
+        <v>2118010.65</v>
       </c>
       <c r="M26" s="128"/>
     </row>
@@ -10175,7 +10214,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -10262,7 +10301,10 @@
         <f>496174*7.12</f>
         <v>3532758.88</v>
       </c>
-      <c r="L2" s="119"/>
+      <c r="L2" s="119">
+        <f>473991*7.1</f>
+        <v>3365336.0999999996</v>
+      </c>
       <c r="M2" s="128"/>
     </row>
     <row r="3" spans="1:13" ht="20.5" customHeight="1">
@@ -10304,7 +10346,10 @@
         <f>129091.37+2727.5+234.28+1417.2</f>
         <v>133470.35</v>
       </c>
-      <c r="L3" s="120"/>
+      <c r="L3" s="120">
+        <f>153537+12710+518+1234+307</f>
+        <v>168306</v>
+      </c>
       <c r="M3" s="128"/>
     </row>
     <row r="4" spans="1:13" ht="20.5" customHeight="1">
@@ -10340,7 +10385,9 @@
       <c r="K4" s="119">
         <v>8461.4</v>
       </c>
-      <c r="L4" s="119"/>
+      <c r="L4" s="119">
+        <v>8176</v>
+      </c>
       <c r="M4" s="128"/>
     </row>
     <row r="5" spans="1:13" ht="20.5" customHeight="1">
@@ -10388,7 +10435,7 @@
       </c>
       <c r="L5" s="122">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3541818.0999999996</v>
       </c>
       <c r="M5" s="128"/>
     </row>
@@ -10431,7 +10478,10 @@
         <f>33429.77+58692.25+27558.72</f>
         <v>119680.73999999999</v>
       </c>
-      <c r="L6" s="119"/>
+      <c r="L6" s="119">
+        <f>33429.77+58692.25+45931.2</f>
+        <v>138053.21999999997</v>
+      </c>
       <c r="M6" s="128"/>
     </row>
     <row r="7" spans="1:13" ht="20.5" customHeight="1">
@@ -10468,7 +10518,9 @@
       <c r="K7" s="119">
         <v>13039</v>
       </c>
-      <c r="L7" s="119"/>
+      <c r="L7" s="119">
+        <v>24142</v>
+      </c>
       <c r="M7" s="128"/>
     </row>
     <row r="8" spans="1:13" ht="20.5" customHeight="1">
@@ -10516,7 +10568,7 @@
       </c>
       <c r="L8" s="124">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>162195.21999999997</v>
       </c>
       <c r="M8" s="128"/>
     </row>
@@ -10648,7 +10700,7 @@
       </c>
       <c r="L12" s="126">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3704013.3199999994</v>
       </c>
       <c r="M12" s="128"/>
     </row>
@@ -10697,7 +10749,7 @@
       </c>
       <c r="L13" s="126">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>3704013.3199999994</v>
       </c>
       <c r="M13" s="128"/>
     </row>
@@ -10749,10 +10801,10 @@
       <c r="B2" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="220" t="s">
+      <c r="C2" s="209" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="221"/>
+      <c r="D2" s="210"/>
       <c r="E2" s="100" t="s">
         <v>51</v>
       </c>
@@ -10785,10 +10837,10 @@
       </c>
     </row>
     <row r="3" spans="2:14" ht="23.5" customHeight="1">
-      <c r="B3" s="200" t="s">
+      <c r="B3" s="211" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="203" t="s">
+      <c r="C3" s="214" t="s">
         <v>62</v>
       </c>
       <c r="D3" s="101" t="s">
@@ -10816,18 +10868,18 @@
       <c r="L3" s="101" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="211">
+      <c r="M3" s="200">
         <f>SUM(J3:J10)</f>
         <v>58430.5</v>
       </c>
-      <c r="N3" s="216">
+      <c r="N3" s="205">
         <f>SUM(M3:M25)</f>
         <v>104966.35</v>
       </c>
     </row>
     <row r="4" spans="2:14" ht="23" customHeight="1">
-      <c r="B4" s="201"/>
-      <c r="C4" s="204"/>
+      <c r="B4" s="212"/>
+      <c r="C4" s="215"/>
       <c r="D4" s="102" t="s">
         <v>70</v>
       </c>
@@ -10851,12 +10903,12 @@
       </c>
       <c r="K4" s="105"/>
       <c r="L4" s="105"/>
-      <c r="M4" s="212"/>
-      <c r="N4" s="217"/>
+      <c r="M4" s="201"/>
+      <c r="N4" s="206"/>
     </row>
     <row r="5" spans="2:14" ht="23" customHeight="1">
-      <c r="B5" s="201"/>
-      <c r="C5" s="205" t="s">
+      <c r="B5" s="212"/>
+      <c r="C5" s="216" t="s">
         <v>74</v>
       </c>
       <c r="D5" s="103" t="s">
@@ -10884,12 +10936,12 @@
       <c r="L5" s="103" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="213"/>
-      <c r="N5" s="218"/>
+      <c r="M5" s="202"/>
+      <c r="N5" s="207"/>
     </row>
     <row r="6" spans="2:14" ht="23" customHeight="1">
-      <c r="B6" s="201"/>
-      <c r="C6" s="204"/>
+      <c r="B6" s="212"/>
+      <c r="C6" s="215"/>
       <c r="D6" s="102" t="s">
         <v>81</v>
       </c>
@@ -10913,11 +10965,11 @@
       </c>
       <c r="K6" s="105"/>
       <c r="L6" s="105"/>
-      <c r="M6" s="212"/>
-      <c r="N6" s="217"/>
+      <c r="M6" s="201"/>
+      <c r="N6" s="206"/>
     </row>
     <row r="7" spans="2:14" ht="23" customHeight="1">
-      <c r="B7" s="201"/>
+      <c r="B7" s="212"/>
       <c r="C7" s="103" t="s">
         <v>87</v>
       </c>
@@ -10944,12 +10996,12 @@
       </c>
       <c r="K7" s="110"/>
       <c r="L7" s="110"/>
-      <c r="M7" s="213"/>
-      <c r="N7" s="218"/>
+      <c r="M7" s="202"/>
+      <c r="N7" s="207"/>
     </row>
     <row r="8" spans="2:14" ht="23" customHeight="1">
-      <c r="B8" s="201"/>
-      <c r="C8" s="206" t="s">
+      <c r="B8" s="212"/>
+      <c r="C8" s="217" t="s">
         <v>92</v>
       </c>
       <c r="D8" s="102" t="s">
@@ -10975,12 +11027,12 @@
       </c>
       <c r="K8" s="105"/>
       <c r="L8" s="105"/>
-      <c r="M8" s="212"/>
-      <c r="N8" s="217"/>
+      <c r="M8" s="201"/>
+      <c r="N8" s="206"/>
     </row>
     <row r="9" spans="2:14" ht="23" customHeight="1">
-      <c r="B9" s="201"/>
-      <c r="C9" s="207"/>
+      <c r="B9" s="212"/>
+      <c r="C9" s="218"/>
       <c r="D9" s="103" t="s">
         <v>97</v>
       </c>
@@ -11004,11 +11056,11 @@
       </c>
       <c r="K9" s="110"/>
       <c r="L9" s="110"/>
-      <c r="M9" s="213"/>
-      <c r="N9" s="218"/>
+      <c r="M9" s="202"/>
+      <c r="N9" s="207"/>
     </row>
     <row r="10" spans="2:14" ht="23.5" customHeight="1">
-      <c r="B10" s="202"/>
+      <c r="B10" s="213"/>
       <c r="C10" s="104" t="s">
         <v>101</v>
       </c>
@@ -11035,14 +11087,14 @@
       </c>
       <c r="K10" s="112"/>
       <c r="L10" s="112"/>
-      <c r="M10" s="214"/>
-      <c r="N10" s="217"/>
+      <c r="M10" s="203"/>
+      <c r="N10" s="206"/>
     </row>
     <row r="11" spans="2:14" ht="23.5" customHeight="1">
-      <c r="B11" s="200" t="s">
+      <c r="B11" s="211" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="203" t="s">
+      <c r="C11" s="214" t="s">
         <v>62</v>
       </c>
       <c r="D11" s="101" t="s">
@@ -11068,15 +11120,15 @@
       </c>
       <c r="K11" s="108"/>
       <c r="L11" s="108"/>
-      <c r="M11" s="211">
+      <c r="M11" s="200">
         <f>SUM(J11:J18)</f>
         <v>9113.5</v>
       </c>
-      <c r="N11" s="218"/>
+      <c r="N11" s="207"/>
     </row>
     <row r="12" spans="2:14" ht="23" customHeight="1">
-      <c r="B12" s="201"/>
-      <c r="C12" s="208"/>
+      <c r="B12" s="212"/>
+      <c r="C12" s="219"/>
       <c r="D12" s="102" t="s">
         <v>70</v>
       </c>
@@ -11100,12 +11152,12 @@
       </c>
       <c r="K12" s="105"/>
       <c r="L12" s="105"/>
-      <c r="M12" s="212"/>
-      <c r="N12" s="217"/>
+      <c r="M12" s="201"/>
+      <c r="N12" s="206"/>
     </row>
     <row r="13" spans="2:14" ht="23" customHeight="1">
-      <c r="B13" s="201"/>
-      <c r="C13" s="209"/>
+      <c r="B13" s="212"/>
+      <c r="C13" s="220"/>
       <c r="D13" s="103" t="s">
         <v>70</v>
       </c>
@@ -11131,12 +11183,12 @@
       <c r="L13" s="103" t="s">
         <v>115</v>
       </c>
-      <c r="M13" s="213"/>
-      <c r="N13" s="218"/>
+      <c r="M13" s="202"/>
+      <c r="N13" s="207"/>
     </row>
     <row r="14" spans="2:14" ht="23" customHeight="1">
-      <c r="B14" s="201"/>
-      <c r="C14" s="206" t="s">
+      <c r="B14" s="212"/>
+      <c r="C14" s="217" t="s">
         <v>74</v>
       </c>
       <c r="D14" s="102" t="s">
@@ -11162,12 +11214,12 @@
       </c>
       <c r="K14" s="105"/>
       <c r="L14" s="105"/>
-      <c r="M14" s="212"/>
-      <c r="N14" s="217"/>
+      <c r="M14" s="201"/>
+      <c r="N14" s="206"/>
     </row>
     <row r="15" spans="2:14" ht="23" customHeight="1">
-      <c r="B15" s="201"/>
-      <c r="C15" s="207"/>
+      <c r="B15" s="212"/>
+      <c r="C15" s="218"/>
       <c r="D15" s="103" t="s">
         <v>75</v>
       </c>
@@ -11191,11 +11243,11 @@
       </c>
       <c r="K15" s="110"/>
       <c r="L15" s="110"/>
-      <c r="M15" s="213"/>
-      <c r="N15" s="218"/>
+      <c r="M15" s="202"/>
+      <c r="N15" s="207"/>
     </row>
     <row r="16" spans="2:14" ht="23" customHeight="1">
-      <c r="B16" s="201"/>
+      <c r="B16" s="212"/>
       <c r="C16" s="102" t="s">
         <v>87</v>
       </c>
@@ -11222,12 +11274,12 @@
       </c>
       <c r="K16" s="105"/>
       <c r="L16" s="105"/>
-      <c r="M16" s="212"/>
-      <c r="N16" s="217"/>
+      <c r="M16" s="201"/>
+      <c r="N16" s="206"/>
     </row>
     <row r="17" spans="2:14" ht="23" customHeight="1">
-      <c r="B17" s="201"/>
-      <c r="C17" s="205" t="s">
+      <c r="B17" s="212"/>
+      <c r="C17" s="216" t="s">
         <v>92</v>
       </c>
       <c r="D17" s="103" t="s">
@@ -11253,12 +11305,12 @@
       </c>
       <c r="K17" s="110"/>
       <c r="L17" s="110"/>
-      <c r="M17" s="213"/>
-      <c r="N17" s="218"/>
+      <c r="M17" s="202"/>
+      <c r="N17" s="207"/>
     </row>
     <row r="18" spans="2:14" ht="23.5" customHeight="1">
-      <c r="B18" s="202"/>
-      <c r="C18" s="208"/>
+      <c r="B18" s="213"/>
+      <c r="C18" s="219"/>
       <c r="D18" s="104" t="s">
         <v>93</v>
       </c>
@@ -11282,14 +11334,14 @@
       </c>
       <c r="K18" s="112"/>
       <c r="L18" s="112"/>
-      <c r="M18" s="214"/>
-      <c r="N18" s="217"/>
+      <c r="M18" s="203"/>
+      <c r="N18" s="206"/>
     </row>
     <row r="19" spans="2:14" ht="23.5" customHeight="1">
-      <c r="B19" s="200" t="s">
+      <c r="B19" s="211" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="203" t="s">
+      <c r="C19" s="214" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="101" t="s">
@@ -11315,15 +11367,15 @@
       </c>
       <c r="K19" s="108"/>
       <c r="L19" s="108"/>
-      <c r="M19" s="211">
+      <c r="M19" s="200">
         <f>SUM(J19:J25)</f>
         <v>37422.35</v>
       </c>
-      <c r="N19" s="218"/>
+      <c r="N19" s="207"/>
     </row>
     <row r="20" spans="2:14" ht="23" customHeight="1">
-      <c r="B20" s="201"/>
-      <c r="C20" s="204"/>
+      <c r="B20" s="212"/>
+      <c r="C20" s="215"/>
       <c r="D20" s="102" t="s">
         <v>70</v>
       </c>
@@ -11347,12 +11399,12 @@
       </c>
       <c r="K20" s="105"/>
       <c r="L20" s="105"/>
-      <c r="M20" s="212"/>
-      <c r="N20" s="217"/>
+      <c r="M20" s="201"/>
+      <c r="N20" s="206"/>
     </row>
     <row r="21" spans="2:14" ht="23" customHeight="1">
-      <c r="B21" s="201"/>
-      <c r="C21" s="205" t="s">
+      <c r="B21" s="212"/>
+      <c r="C21" s="216" t="s">
         <v>74</v>
       </c>
       <c r="D21" s="103" t="s">
@@ -11378,12 +11430,12 @@
       </c>
       <c r="K21" s="110"/>
       <c r="L21" s="110"/>
-      <c r="M21" s="213"/>
-      <c r="N21" s="218"/>
+      <c r="M21" s="202"/>
+      <c r="N21" s="207"/>
     </row>
     <row r="22" spans="2:14" ht="23" customHeight="1">
-      <c r="B22" s="201"/>
-      <c r="C22" s="210"/>
+      <c r="B22" s="212"/>
+      <c r="C22" s="221"/>
       <c r="D22" s="102" t="s">
         <v>132</v>
       </c>
@@ -11407,12 +11459,12 @@
       </c>
       <c r="K22" s="105"/>
       <c r="L22" s="105"/>
-      <c r="M22" s="212"/>
-      <c r="N22" s="217"/>
+      <c r="M22" s="201"/>
+      <c r="N22" s="206"/>
     </row>
     <row r="23" spans="2:14" ht="23" customHeight="1">
-      <c r="B23" s="201"/>
-      <c r="C23" s="205" t="s">
+      <c r="B23" s="212"/>
+      <c r="C23" s="216" t="s">
         <v>92</v>
       </c>
       <c r="D23" s="103" t="s">
@@ -11438,12 +11490,12 @@
       </c>
       <c r="K23" s="110"/>
       <c r="L23" s="110"/>
-      <c r="M23" s="213"/>
-      <c r="N23" s="218"/>
+      <c r="M23" s="202"/>
+      <c r="N23" s="207"/>
     </row>
     <row r="24" spans="2:14" ht="23" customHeight="1">
-      <c r="B24" s="201"/>
-      <c r="C24" s="204"/>
+      <c r="B24" s="212"/>
+      <c r="C24" s="215"/>
       <c r="D24" s="102" t="s">
         <v>97</v>
       </c>
@@ -11467,11 +11519,11 @@
       </c>
       <c r="K24" s="105"/>
       <c r="L24" s="105"/>
-      <c r="M24" s="212"/>
-      <c r="N24" s="217"/>
+      <c r="M24" s="201"/>
+      <c r="N24" s="206"/>
     </row>
     <row r="25" spans="2:14" ht="23.5" customHeight="1">
-      <c r="B25" s="202"/>
+      <c r="B25" s="213"/>
       <c r="C25" s="106" t="s">
         <v>101</v>
       </c>
@@ -11500,16 +11552,11 @@
       <c r="L25" s="106" t="s">
         <v>143</v>
       </c>
-      <c r="M25" s="215"/>
-      <c r="N25" s="219"/>
+      <c r="M25" s="204"/>
+      <c r="N25" s="208"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="M3:M10"/>
-    <mergeCell ref="M11:M18"/>
-    <mergeCell ref="M19:M25"/>
-    <mergeCell ref="N3:N25"/>
-    <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B10"/>
     <mergeCell ref="B11:B18"/>
     <mergeCell ref="B19:B25"/>
@@ -11522,6 +11569,11 @@
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C23:C24"/>
+    <mergeCell ref="M3:M10"/>
+    <mergeCell ref="M11:M18"/>
+    <mergeCell ref="M19:M25"/>
+    <mergeCell ref="N3:N25"/>
+    <mergeCell ref="C2:D2"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -13196,39 +13248,39 @@
   <sheetData>
     <row r="1" spans="2:30" ht="31" customHeight="1"/>
     <row r="2" spans="2:30" ht="25" customHeight="1">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="240" t="s">
         <v>295</v>
       </c>
-      <c r="C2" s="222"/>
+      <c r="C2" s="240"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="I2" s="222" t="s">
+      <c r="I2" s="240" t="s">
         <v>296</v>
       </c>
-      <c r="J2" s="222"/>
-      <c r="K2" s="222"/>
-      <c r="L2" s="222"/>
-      <c r="M2" s="222"/>
-      <c r="N2" s="222"/>
-      <c r="Q2" s="222" t="s">
+      <c r="J2" s="240"/>
+      <c r="K2" s="240"/>
+      <c r="L2" s="240"/>
+      <c r="M2" s="240"/>
+      <c r="N2" s="240"/>
+      <c r="Q2" s="240" t="s">
         <v>297</v>
       </c>
-      <c r="R2" s="222"/>
-      <c r="S2" s="222"/>
-      <c r="T2" s="222"/>
-      <c r="U2" s="222"/>
-      <c r="V2" s="222"/>
-      <c r="W2" s="222"/>
-      <c r="Y2" s="222" t="s">
+      <c r="R2" s="240"/>
+      <c r="S2" s="240"/>
+      <c r="T2" s="240"/>
+      <c r="U2" s="240"/>
+      <c r="V2" s="240"/>
+      <c r="W2" s="240"/>
+      <c r="Y2" s="240" t="s">
         <v>298</v>
       </c>
-      <c r="Z2" s="222"/>
-      <c r="AA2" s="222"/>
-      <c r="AB2" s="222"/>
-      <c r="AC2" s="222"/>
-      <c r="AD2" s="222"/>
+      <c r="Z2" s="240"/>
+      <c r="AA2" s="240"/>
+      <c r="AB2" s="240"/>
+      <c r="AC2" s="240"/>
+      <c r="AD2" s="240"/>
     </row>
     <row r="3" spans="2:30" ht="20" customHeight="1">
       <c r="B3" s="3" t="s">
@@ -13310,7 +13362,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="I4" s="236" t="s">
+      <c r="I4" s="229" t="s">
         <v>317</v>
       </c>
       <c r="J4" s="47" t="s">
@@ -13319,14 +13371,14 @@
       <c r="K4" s="48">
         <v>13000</v>
       </c>
-      <c r="L4" s="242">
+      <c r="L4" s="235">
         <f>SUM(K4:K8)</f>
         <v>13000</v>
       </c>
       <c r="M4" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="N4" s="223">
+      <c r="N4" s="241">
         <f>L4/J14</f>
         <v>0.56521739130434778</v>
       </c>
@@ -13390,18 +13442,18 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="I5" s="237"/>
+      <c r="I5" s="230"/>
       <c r="J5" s="47" t="s">
         <v>320</v>
       </c>
       <c r="K5" s="48">
         <v>0</v>
       </c>
-      <c r="L5" s="224"/>
+      <c r="L5" s="236"/>
       <c r="M5" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="N5" s="224"/>
+      <c r="N5" s="236"/>
       <c r="Q5" s="63" t="s">
         <v>254</v>
       </c>
@@ -13465,16 +13517,16 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="I6" s="238"/>
+      <c r="I6" s="231"/>
       <c r="J6" s="47" t="s">
         <v>322</v>
       </c>
       <c r="K6" s="49"/>
-      <c r="L6" s="225"/>
+      <c r="L6" s="237"/>
       <c r="M6" s="54">
         <v>582000</v>
       </c>
-      <c r="N6" s="225"/>
+      <c r="N6" s="237"/>
       <c r="Q6" s="63" t="s">
         <v>256</v>
       </c>
@@ -13539,16 +13591,16 @@
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
-      <c r="I7" s="239"/>
+      <c r="I7" s="232"/>
       <c r="J7" s="47" t="s">
         <v>324</v>
       </c>
       <c r="K7" s="48">
         <v>0</v>
       </c>
-      <c r="L7" s="226"/>
+      <c r="L7" s="238"/>
       <c r="M7" s="55"/>
-      <c r="N7" s="226"/>
+      <c r="N7" s="238"/>
       <c r="Q7" s="63" t="s">
         <v>258</v>
       </c>
@@ -13612,14 +13664,14 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="I8" s="239"/>
+      <c r="I8" s="232"/>
       <c r="J8" s="47" t="s">
         <v>326</v>
       </c>
       <c r="K8" s="49"/>
-      <c r="L8" s="226"/>
+      <c r="L8" s="238"/>
       <c r="M8" s="55"/>
-      <c r="N8" s="226"/>
+      <c r="N8" s="238"/>
       <c r="Q8" s="63" t="s">
         <v>260</v>
       </c>
@@ -13673,21 +13725,21 @@
       </c>
     </row>
     <row r="9" spans="2:30" ht="20" customHeight="1">
-      <c r="I9" s="236" t="s">
+      <c r="I9" s="229" t="s">
         <v>327</v>
       </c>
       <c r="J9" s="47" t="s">
         <v>328</v>
       </c>
       <c r="K9" s="49"/>
-      <c r="L9" s="243">
+      <c r="L9" s="239">
         <f>SUM(K9:K13)</f>
         <v>10000</v>
       </c>
       <c r="M9" s="54">
         <v>1000000</v>
       </c>
-      <c r="N9" s="227">
+      <c r="N9" s="242">
         <f>L9/J14</f>
         <v>0.43478260869565216</v>
       </c>
@@ -13744,18 +13796,18 @@
       </c>
     </row>
     <row r="10" spans="2:30" ht="20" customHeight="1">
-      <c r="I10" s="240"/>
+      <c r="I10" s="233"/>
       <c r="J10" s="47" t="s">
         <v>329</v>
       </c>
       <c r="K10" s="48">
         <v>0</v>
       </c>
-      <c r="L10" s="224"/>
+      <c r="L10" s="236"/>
       <c r="M10" s="54">
         <v>400000</v>
       </c>
-      <c r="N10" s="224"/>
+      <c r="N10" s="236"/>
       <c r="Q10" s="63" t="s">
         <v>264</v>
       </c>
@@ -13809,18 +13861,18 @@
       </c>
     </row>
     <row r="11" spans="2:30" ht="20" customHeight="1">
-      <c r="I11" s="240"/>
+      <c r="I11" s="233"/>
       <c r="J11" s="47" t="s">
         <v>330</v>
       </c>
       <c r="K11" s="50">
         <v>10000</v>
       </c>
-      <c r="L11" s="224"/>
+      <c r="L11" s="236"/>
       <c r="M11" s="56">
         <v>2000000</v>
       </c>
-      <c r="N11" s="224"/>
+      <c r="N11" s="236"/>
       <c r="Q11" s="63" t="s">
         <v>266</v>
       </c>
@@ -13874,24 +13926,24 @@
       </c>
     </row>
     <row r="12" spans="2:30" ht="20" customHeight="1">
-      <c r="B12" s="222" t="s">
+      <c r="B12" s="240" t="s">
         <v>331</v>
       </c>
-      <c r="C12" s="222"/>
-      <c r="D12" s="222"/>
-      <c r="E12" s="222"/>
-      <c r="F12" s="222"/>
-      <c r="G12" s="222"/>
-      <c r="I12" s="240"/>
+      <c r="C12" s="240"/>
+      <c r="D12" s="240"/>
+      <c r="E12" s="240"/>
+      <c r="F12" s="240"/>
+      <c r="G12" s="240"/>
+      <c r="I12" s="233"/>
       <c r="J12" s="47" t="s">
         <v>332</v>
       </c>
       <c r="K12" s="48">
         <v>0</v>
       </c>
-      <c r="L12" s="224"/>
+      <c r="L12" s="236"/>
       <c r="M12" s="55"/>
-      <c r="N12" s="224"/>
+      <c r="N12" s="236"/>
       <c r="Q12" s="63" t="s">
         <v>268</v>
       </c>
@@ -13963,16 +14015,16 @@
       <c r="G13" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="I13" s="241"/>
+      <c r="I13" s="234"/>
       <c r="J13" s="51" t="s">
         <v>338</v>
       </c>
       <c r="K13" s="51" t="s">
         <v>338</v>
       </c>
-      <c r="L13" s="225"/>
+      <c r="L13" s="237"/>
       <c r="M13" s="55"/>
-      <c r="N13" s="228"/>
+      <c r="N13" s="243"/>
       <c r="Q13" s="63" t="s">
         <v>270</v>
       </c>
@@ -14049,12 +14101,12 @@
       <c r="I14" s="52" t="s">
         <v>339</v>
       </c>
-      <c r="J14" s="229">
+      <c r="J14" s="222">
         <f>SUM(K4:K13)</f>
         <v>23000</v>
       </c>
-      <c r="K14" s="230"/>
-      <c r="L14" s="231"/>
+      <c r="K14" s="223"/>
+      <c r="L14" s="224"/>
       <c r="M14" s="57">
         <f>SUM(M5:M11)</f>
         <v>3982000</v>
@@ -14137,12 +14189,12 @@
       <c r="I15" s="52" t="s">
         <v>340</v>
       </c>
-      <c r="J15" s="229">
+      <c r="J15" s="222">
         <f>J14/C7</f>
         <v>5321.681319084737</v>
       </c>
-      <c r="K15" s="230"/>
-      <c r="L15" s="232"/>
+      <c r="K15" s="223"/>
+      <c r="L15" s="225"/>
       <c r="M15" s="55"/>
       <c r="N15" s="59"/>
       <c r="Q15" s="63" t="s">
@@ -14222,13 +14274,13 @@
       <c r="I16" s="52" t="s">
         <v>341</v>
       </c>
-      <c r="J16" s="233">
+      <c r="J16" s="226">
         <f>J14/C7</f>
         <v>5321.681319084737</v>
       </c>
-      <c r="K16" s="234"/>
-      <c r="L16" s="234"/>
-      <c r="M16" s="235"/>
+      <c r="K16" s="227"/>
+      <c r="L16" s="227"/>
+      <c r="M16" s="228"/>
       <c r="N16" s="60"/>
       <c r="Q16" s="63" t="s">
         <v>276</v>
@@ -15621,6 +15673,13 @@
     <row r="110" ht="26.4" customHeight="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="Y2:AD2"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="N4:N8"/>
+    <mergeCell ref="N9:N13"/>
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="J16:M16"/>
@@ -15628,13 +15687,6 @@
     <mergeCell ref="I9:I13"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L9:L13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="Q2:W2"/>
-    <mergeCell ref="Y2:AD2"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="N4:N8"/>
-    <mergeCell ref="N9:N13"/>
   </mergeCells>
   <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>